<commit_message>
Update Product.xlsx : Tested write operation on this file
</commit_message>
<xml_diff>
--- a/product.xlsx
+++ b/product.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t/>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>List</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
   <si>
     <t>Orange Juice</t>
@@ -104,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -115,6 +118,7 @@
     <col min="3" max="3" width="10.0" customWidth="true"/>
     <col min="4" max="4" width="8.0" customWidth="true"/>
     <col min="5" max="5" width="8.0" customWidth="true"/>
+    <col min="6" max="6" width="16.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -133,13 +137,16 @@
       <c r="E1" t="s" s="1">
         <v>5</v>
       </c>
+      <c r="F1" t="s" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="n" s="0">
         <v>10.0</v>
@@ -148,15 +155,18 @@
         <v>42282.0</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>10.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n" s="0">
         <v>20.0</v>
@@ -165,15 +175,18 @@
         <v>42282.0</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>5.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="n" s="0">
         <v>15.0</v>
@@ -182,7 +195,10 @@
         <v>42282.0</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>7.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>